<commit_message>
re structure the databases
</commit_message>
<xml_diff>
--- a/test/fixtures/signatories.xlsx
+++ b/test/fixtures/signatories.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="24960" windowHeight="15060"/>
   </bookViews>
   <sheets>
     <sheet name="OR" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="213">
   <si>
     <t>FIELD OFFICE</t>
   </si>
@@ -662,6 +662,9 @@
   </si>
   <si>
     <t>DEPARTMENT OF SOCIAL WELFARE AND DEVELOPMENT</t>
+  </si>
+  <si>
+    <t>XIII</t>
   </si>
 </sst>
 </file>
@@ -1503,8 +1506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3247,7 +3250,7 @@
     </row>
     <row r="97" spans="2:15" ht="15">
       <c r="B97" s="20" t="s">
-        <v>21</v>
+        <v>212</v>
       </c>
       <c r="C97" s="71" t="s">
         <v>186</v>
@@ -3505,7 +3508,6 @@
     <mergeCell ref="C6:H6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.5" bottom="0.25" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" orientation="landscape"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5525,7 +5527,6 @@
     <mergeCell ref="C7:M7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0" top="0.5" bottom="0" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" orientation="landscape"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>